<commit_message>
update font sizes excel
</commit_message>
<xml_diff>
--- a/0_dev/00_font-sizes.xlsx
+++ b/0_dev/00_font-sizes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awisnicki2/GitHub/undiscipliningvc/0_dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08D96D53-CCE6-CD48-AC77-3FAE8691B499}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BC43AC-7DF4-6646-A8A5-4F99CF17CFEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="460" windowWidth="24960" windowHeight="15000" xr2:uid="{DEC15694-0F7D-A642-B9F4-9D4C39EDC236}"/>
+    <workbookView xWindow="580" yWindow="460" windowWidth="24960" windowHeight="15000" xr2:uid="{DEC15694-0F7D-A642-B9F4-9D4C39EDC236}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,7 +439,7 @@
   <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -519,13 +519,10 @@
         <v>1.3</v>
       </c>
       <c r="C9">
-        <v>1.6</v>
+        <v>1.7</v>
       </c>
       <c r="D9">
-        <v>1.9</v>
-      </c>
-      <c r="E9">
-        <v>2.1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -533,7 +530,7 @@
         <v>7</v>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>